<commit_message>
chore: fix image tests
</commit_message>
<xml_diff>
--- a/test/expected/insert_image.xlsx
+++ b/test/expected/insert_image.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -72,7 +72,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="rust logo"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>

<commit_message>
feat: add image methods (#95)
* chore: refactor object_movement

* feat: add image methods

* chore: fix image tests
</commit_message>
<xml_diff>
--- a/test/expected/insert_image.xlsx
+++ b/test/expected/insert_image.xlsx
@@ -57,7 +57,7 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -72,7 +72,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="rust logo"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>

</xml_diff>